<commit_message>
Tried to fix the freq
</commit_message>
<xml_diff>
--- a/input/rfims.xlsx
+++ b/input/rfims.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="8890" yWindow="2780" windowWidth="2970" windowHeight="1550" activeTab="5"/>
+    <workbookView xWindow="8890" yWindow="2780" windowWidth="2970" windowHeight="1550" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
@@ -12,14 +12,13 @@
     <sheet name="Sheet3" sheetId="7" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="8" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="9" r:id="rId5"/>
-    <sheet name="Sheet6" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="95">
   <si>
     <t>Parent</t>
   </si>
@@ -27,27 +26,12 @@
     <t>Block</t>
   </si>
   <si>
-    <t>cns</t>
-  </si>
-  <si>
     <t>software</t>
   </si>
   <si>
-    <t>rfs</t>
-  </si>
-  <si>
     <t>firmware</t>
   </si>
   <si>
-    <t>rrfs</t>
-  </si>
-  <si>
-    <t>scs</t>
-  </si>
-  <si>
-    <t>sdri</t>
-  </si>
-  <si>
     <t>power</t>
   </si>
   <si>
@@ -112,9 +96,6 @@
   </si>
   <si>
     <t>sdri_input</t>
-  </si>
-  <si>
-    <t>Grandparent</t>
   </si>
   <si>
     <t>MTBM.CM</t>
@@ -701,39 +682,39 @@
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="I1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="J1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="K1" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B2">
         <v>1000000</v>
@@ -763,12 +744,12 @@
         <v>30</v>
       </c>
       <c r="K2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B3" s="3">
         <v>1000000</v>
@@ -798,12 +779,12 @@
         <v>30</v>
       </c>
       <c r="K3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B4">
         <v>100000</v>
@@ -833,12 +814,12 @@
         <v>30</v>
       </c>
       <c r="K4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B5">
         <v>50000</v>
@@ -868,12 +849,12 @@
         <v>30</v>
       </c>
       <c r="K5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B6">
         <f>ROUND(1000000000/6006,0)</f>
@@ -904,12 +885,12 @@
         <v>30</v>
       </c>
       <c r="K6" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B7">
         <v>199748</v>
@@ -939,12 +920,12 @@
         <v>30</v>
       </c>
       <c r="K7" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B8">
         <v>666667000</v>
@@ -974,12 +955,12 @@
         <v>30</v>
       </c>
       <c r="K8" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B9">
         <v>281530</v>
@@ -1009,12 +990,12 @@
         <v>30</v>
       </c>
       <c r="K9" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B10">
         <v>1619997</v>
@@ -1044,12 +1025,12 @@
         <v>30</v>
       </c>
       <c r="K10" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B11">
         <f>ROUND(1000000000/6667,0)</f>
@@ -1080,12 +1061,12 @@
         <v>30</v>
       </c>
       <c r="K11" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B12">
         <v>120870</v>
@@ -1115,12 +1096,12 @@
         <v>30</v>
       </c>
       <c r="K12" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B13">
         <f>ROUND(1000000000/31771,0)</f>
@@ -1151,12 +1132,12 @@
         <v>30</v>
       </c>
       <c r="K13" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B14">
         <f>ROUND(1000000000/5000,0)</f>
@@ -1187,12 +1168,12 @@
         <v>30</v>
       </c>
       <c r="K14" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B15">
         <f>ROUND(1000000000/5000,0)</f>
@@ -1223,12 +1204,12 @@
         <v>30</v>
       </c>
       <c r="K15" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B16">
         <v>15602810</v>
@@ -1258,12 +1239,12 @@
         <v>30</v>
       </c>
       <c r="K16" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B17">
         <v>15825</v>
@@ -1293,12 +1274,12 @@
         <v>30</v>
       </c>
       <c r="K17" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B18">
         <v>100000</v>
@@ -1328,12 +1309,12 @@
         <v>30</v>
       </c>
       <c r="K18" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B19">
         <f>ROUND(1000000000/7135,0)</f>
@@ -1364,12 +1345,12 @@
         <v>30</v>
       </c>
       <c r="K19" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B20">
         <v>160000</v>
@@ -1399,12 +1380,12 @@
         <v>30</v>
       </c>
       <c r="K20" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B21">
         <v>208000</v>
@@ -1434,12 +1415,12 @@
         <v>30</v>
       </c>
       <c r="K21" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B22">
         <v>576450</v>
@@ -1469,12 +1450,12 @@
         <v>30</v>
       </c>
       <c r="K22" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B23">
         <v>117523</v>
@@ -1504,12 +1485,12 @@
         <v>30</v>
       </c>
       <c r="K23" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B24">
         <v>121356</v>
@@ -1539,12 +1520,12 @@
         <v>30</v>
       </c>
       <c r="K24" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B25">
         <v>208000</v>
@@ -1574,12 +1555,12 @@
         <v>30</v>
       </c>
       <c r="K25" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B26">
         <v>60000</v>
@@ -1609,12 +1590,12 @@
         <v>30</v>
       </c>
       <c r="K26" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B27">
         <v>100000</v>
@@ -1644,12 +1625,12 @@
         <v>30</v>
       </c>
       <c r="K27" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B28">
         <v>62627</v>
@@ -1679,12 +1660,12 @@
         <v>30</v>
       </c>
       <c r="K28" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B29">
         <f>ROUND(1000000000/17544,0)</f>
@@ -1715,12 +1696,12 @@
         <v>30</v>
       </c>
       <c r="K29" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B30">
         <v>120870</v>
@@ -1750,12 +1731,12 @@
         <v>30</v>
       </c>
       <c r="K30" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B31">
         <v>120870</v>
@@ -1785,12 +1766,12 @@
         <v>30</v>
       </c>
       <c r="K31" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B32">
         <v>6521736</v>
@@ -1820,12 +1801,12 @@
         <v>30</v>
       </c>
       <c r="K32" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B33">
         <f>ROUND(1000000000/31771,0)</f>
@@ -1856,12 +1837,12 @@
         <v>30</v>
       </c>
       <c r="K33" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B34" s="3">
         <v>5030000000</v>
@@ -1891,12 +1872,12 @@
         <v>30</v>
       </c>
       <c r="K34" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B35" s="3">
         <v>3390000</v>
@@ -1926,12 +1907,12 @@
         <v>30</v>
       </c>
       <c r="K35" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B36" s="3">
         <v>7400000</v>
@@ -1961,12 +1942,12 @@
         <v>30</v>
       </c>
       <c r="K36" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B37">
         <f>ROUND(1000000000/31771,0)</f>
@@ -1997,12 +1978,12 @@
         <v>30</v>
       </c>
       <c r="K37" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B38">
         <v>1200</v>
@@ -2032,12 +2013,12 @@
         <v>30</v>
       </c>
       <c r="K38" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B39">
         <f>ROUND(1000000000/63191,0)</f>
@@ -2068,12 +2049,12 @@
         <v>30</v>
       </c>
       <c r="K39" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B40">
         <f>ROUND(1000000000/11658,0)</f>
@@ -2104,12 +2085,12 @@
         <v>30</v>
       </c>
       <c r="K40" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B41">
         <v>757795</v>
@@ -2139,12 +2120,12 @@
         <v>30</v>
       </c>
       <c r="K41" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B42" s="3">
         <v>1000000</v>
@@ -2174,7 +2155,7 @@
         <v>30</v>
       </c>
       <c r="K42" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.35">
@@ -2261,18 +2242,18 @@
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C2">
         <v>15</v>
@@ -2283,10 +2264,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C3">
         <v>45</v>
@@ -2297,10 +2278,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C4">
         <v>15</v>
@@ -2311,10 +2292,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -2325,10 +2306,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C6">
         <v>15</v>
@@ -2339,10 +2320,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -2353,10 +2334,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -2367,10 +2348,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B9" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -2381,10 +2362,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -2395,10 +2376,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -2409,10 +2390,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -2423,10 +2404,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -2437,10 +2418,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -2451,10 +2432,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -2465,10 +2446,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -2479,10 +2460,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -2493,10 +2474,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B18" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -2507,10 +2488,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -2521,10 +2502,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B20" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -2535,10 +2516,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B21" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -2549,10 +2530,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -2563,10 +2544,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B23" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -2577,10 +2558,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B24" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -2591,10 +2572,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -2605,10 +2586,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B26" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -2619,10 +2600,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B27" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -2633,10 +2614,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B28" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -2647,10 +2628,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -2661,10 +2642,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B30" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -2675,10 +2656,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B31" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C31">
         <v>2</v>
@@ -2689,10 +2670,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B32" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -2703,10 +2684,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B33" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -2717,10 +2698,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B34" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -2731,10 +2712,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -2745,10 +2726,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B36" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -2759,10 +2740,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B37" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -2773,10 +2754,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B38" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -2787,10 +2768,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B39" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -2801,10 +2782,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B40" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C40">
         <v>3</v>
@@ -2841,18 +2822,18 @@
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -2863,10 +2844,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -2877,10 +2858,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -2891,10 +2872,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -2905,10 +2886,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -2919,10 +2900,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -2933,10 +2914,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C8">
         <v>3</v>
@@ -2947,10 +2928,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -2961,10 +2942,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B10" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C10">
         <v>3</v>
@@ -2975,10 +2956,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B11" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -2989,10 +2970,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -3003,10 +2984,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B13" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C13">
         <v>3</v>
@@ -3017,10 +2998,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B14" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C14">
         <v>3</v>
@@ -3031,10 +3012,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B15" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -3045,10 +3026,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B16" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C16">
         <v>8</v>
@@ -3059,10 +3040,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B17" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -3073,10 +3054,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B18" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -3114,18 +3095,18 @@
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -3136,10 +3117,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -3150,10 +3131,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -3164,10 +3145,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -3178,10 +3159,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -3192,10 +3173,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -3206,10 +3187,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -3220,10 +3201,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -3234,10 +3215,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C10">
         <v>16</v>
@@ -3248,10 +3229,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -3262,10 +3243,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -3276,10 +3257,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -3290,10 +3271,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C14">
         <v>3</v>
@@ -3304,10 +3285,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -3318,10 +3299,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C16">
         <v>4</v>
@@ -3332,10 +3313,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -3346,10 +3327,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -3360,10 +3341,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -3374,10 +3355,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -3388,10 +3369,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -3402,10 +3383,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C22">
         <v>3</v>
@@ -3416,10 +3397,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C23">
         <v>16</v>
@@ -3430,10 +3411,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -3444,10 +3425,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -3458,10 +3439,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -3472,10 +3453,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B27" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C27">
         <v>3</v>
@@ -3486,10 +3467,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B28" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -3500,10 +3481,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C29">
         <v>4</v>
@@ -3514,10 +3495,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -3528,10 +3509,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -3542,10 +3523,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B32" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -3556,10 +3537,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B33" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -3570,10 +3551,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B34" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -3584,10 +3565,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B35" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -3598,10 +3579,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B36" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -3612,10 +3593,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B37" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -3626,10 +3607,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B38" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C38">
         <v>5</v>
@@ -3640,10 +3621,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B39" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -3654,10 +3635,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B40" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -3668,10 +3649,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B41" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -3682,10 +3663,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B42" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -3696,10 +3677,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B43" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -3710,10 +3691,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B44" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -3724,10 +3705,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B45" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -3745,7 +3726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -3764,18 +3745,18 @@
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -3786,10 +3767,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -3800,10 +3781,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -3814,10 +3795,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -3828,10 +3809,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -3842,10 +3823,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -3856,10 +3837,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -3870,10 +3851,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -3884,10 +3865,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B10" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -3898,10 +3879,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -3912,10 +3893,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -3927,800 +3908,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I26"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="30.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.81640625" customWidth="1"/>
-    <col min="4" max="4" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="9" width="21.453125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>199748</v>
-      </c>
-      <c r="G2">
-        <v>4320</v>
-      </c>
-      <c r="H2">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>281530</v>
-      </c>
-      <c r="G3">
-        <v>4320</v>
-      </c>
-      <c r="H3">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4">
-        <v>62627</v>
-      </c>
-      <c r="G4">
-        <v>4320</v>
-      </c>
-      <c r="H4">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>6</v>
-      </c>
-      <c r="E5">
-        <v>7</v>
-      </c>
-      <c r="F5">
-        <v>5600</v>
-      </c>
-      <c r="G5">
-        <v>4320</v>
-      </c>
-      <c r="H5">
-        <v>0.75</v>
-      </c>
-      <c r="I5">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>120870</v>
-      </c>
-      <c r="G6">
-        <f>24*30*12</f>
-        <v>8640</v>
-      </c>
-      <c r="H6">
-        <v>24</v>
-      </c>
-      <c r="I6">
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>15699.769391896119</v>
-      </c>
-      <c r="G7">
-        <f>24*30*12</f>
-        <v>8640</v>
-      </c>
-      <c r="H7">
-        <v>24</v>
-      </c>
-      <c r="I7">
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>200000</v>
-      </c>
-      <c r="G8">
-        <f>24*30*12</f>
-        <v>8640</v>
-      </c>
-      <c r="H8">
-        <v>32</v>
-      </c>
-      <c r="I8">
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>200000</v>
-      </c>
-      <c r="G9">
-        <f>24*30*12</f>
-        <v>8640</v>
-      </c>
-      <c r="H9">
-        <v>32</v>
-      </c>
-      <c r="I9">
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>2</v>
-      </c>
-      <c r="F10">
-        <v>199748</v>
-      </c>
-      <c r="G10">
-        <v>4320</v>
-      </c>
-      <c r="H10">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
-      <c r="F11">
-        <v>281530</v>
-      </c>
-      <c r="G11">
-        <v>4320</v>
-      </c>
-      <c r="H11">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>2</v>
-      </c>
-      <c r="F12">
-        <v>62627</v>
-      </c>
-      <c r="G12">
-        <v>4320</v>
-      </c>
-      <c r="H12">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>15699.769391896119</v>
-      </c>
-      <c r="G13">
-        <f>24*30*12</f>
-        <v>8640</v>
-      </c>
-      <c r="H13">
-        <v>24</v>
-      </c>
-      <c r="I13">
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14">
-        <v>200000</v>
-      </c>
-      <c r="G14">
-        <f>24*30*12</f>
-        <v>8640</v>
-      </c>
-      <c r="H14">
-        <v>32</v>
-      </c>
-      <c r="I14">
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15">
-        <v>200000</v>
-      </c>
-      <c r="G15">
-        <f>24*30*12</f>
-        <v>8640</v>
-      </c>
-      <c r="H15">
-        <v>32</v>
-      </c>
-      <c r="I15">
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16">
-        <v>120870</v>
-      </c>
-      <c r="G16">
-        <f>24*30*12</f>
-        <v>8640</v>
-      </c>
-      <c r="H16">
-        <v>24</v>
-      </c>
-      <c r="I16">
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17">
-        <v>2</v>
-      </c>
-      <c r="F17">
-        <v>199748</v>
-      </c>
-      <c r="G17">
-        <v>4320</v>
-      </c>
-      <c r="H17">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="I17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18">
-        <v>2</v>
-      </c>
-      <c r="F18">
-        <v>281530</v>
-      </c>
-      <c r="G18">
-        <v>4320</v>
-      </c>
-      <c r="H18">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="I18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>2</v>
-      </c>
-      <c r="F19">
-        <v>62627</v>
-      </c>
-      <c r="G19">
-        <v>4320</v>
-      </c>
-      <c r="H19">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="I19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20">
-        <v>5</v>
-      </c>
-      <c r="E20">
-        <v>6</v>
-      </c>
-      <c r="F20">
-        <v>5600</v>
-      </c>
-      <c r="G20">
-        <v>4320</v>
-      </c>
-      <c r="H20">
-        <v>0.75</v>
-      </c>
-      <c r="I20">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="F21">
-        <v>149993</v>
-      </c>
-      <c r="G21">
-        <v>4320</v>
-      </c>
-      <c r="H21">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="I21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22">
-        <v>120870</v>
-      </c>
-      <c r="G22">
-        <f>24*30*12</f>
-        <v>8640</v>
-      </c>
-      <c r="H22">
-        <v>24</v>
-      </c>
-      <c r="I22">
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-      <c r="F23">
-        <v>31475</v>
-      </c>
-      <c r="G23">
-        <f>24*30*12</f>
-        <v>8640</v>
-      </c>
-      <c r="H23">
-        <v>24</v>
-      </c>
-      <c r="I23">
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-      <c r="F24">
-        <v>200000</v>
-      </c>
-      <c r="G24">
-        <f>24*30*12</f>
-        <v>8640</v>
-      </c>
-      <c r="H24">
-        <v>32</v>
-      </c>
-      <c r="I24">
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-      <c r="F25">
-        <v>57000</v>
-      </c>
-      <c r="G25">
-        <f>24*30*12</f>
-        <v>8640</v>
-      </c>
-      <c r="H25">
-        <v>32</v>
-      </c>
-      <c r="I25">
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="F26">
-        <v>31475</v>
-      </c>
-      <c r="G26">
-        <f>24*30*12</f>
-        <v>8640</v>
-      </c>
-      <c r="H26">
-        <v>32</v>
-      </c>
-      <c r="I26">
-        <v>2.4</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState ref="A2:I26">
-    <sortCondition ref="B2:B26"/>
-    <sortCondition ref="A2:A26"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>